<commit_message>
fix compile bugs in unity
</commit_message>
<xml_diff>
--- a/挂机游戏表格.xlsx
+++ b/挂机游戏表格.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyProjects\code\src\github.com\ddiay\go-xlsx2code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Unity\NonStop\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="7095" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="7095" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterClass" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Scene" sheetId="5" r:id="rId3"/>
     <sheet name="RespawnPoint" sheetId="8" r:id="rId4"/>
     <sheet name="UnitGroup" sheetId="6" r:id="rId5"/>
-    <sheet name="Exp" sheetId="3" r:id="rId6"/>
+    <sheet name="LevelUp" sheetId="3" r:id="rId6"/>
     <sheet name="Skin" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -431,6 +431,10 @@
   </si>
   <si>
     <t>单位组列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lev</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1205,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -1599,7 +1603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1610,7 +1614,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
@@ -1715,6 +1719,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix compile error, add u3d package
</commit_message>
<xml_diff>
--- a/挂机游戏表格.xlsx
+++ b/挂机游戏表格.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="7095" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="7095" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterClass" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="120">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,10 +108,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"body":1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>射手</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -140,10 +136,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"body":2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>怪物1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,18 +148,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"body":3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"body":4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"body":5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Exp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -316,125 +296,191 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RandomOrOrder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机组（随机或是按顺序）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body1.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body2.prefab</t>
+  </si>
+  <si>
+    <t>body3.prefab</t>
+  </si>
+  <si>
+    <t>body4.prefab</t>
+  </si>
+  <si>
+    <t>body5.prefab</t>
+  </si>
+  <si>
+    <t>body6.prefab</t>
+  </si>
+  <si>
+    <t>body7.prefab</t>
+  </si>
+  <si>
+    <t>body8.prefab</t>
+  </si>
+  <si>
+    <t>Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body2</t>
+  </si>
+  <si>
+    <t>body3</t>
+  </si>
+  <si>
+    <t>body4</t>
+  </si>
+  <si>
+    <t>body5</t>
+  </si>
+  <si>
+    <t>body6</t>
+  </si>
+  <si>
+    <t>body7</t>
+  </si>
+  <si>
+    <t>body8</t>
+  </si>
+  <si>
+    <t>#number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[RespawnPoint.Id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[string:Skin.Id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharacterClass.Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[UnitGroup.Id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Unit.Id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位组列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重生点1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重生点2</t>
+  </si>
+  <si>
+    <t>重生点3</t>
+  </si>
+  <si>
+    <t>重生点4</t>
+  </si>
+  <si>
+    <t>重生点5</t>
+  </si>
+  <si>
+    <t>重生点6</t>
+  </si>
+  <si>
+    <t>重生点7</t>
+  </si>
+  <si>
     <t>4,5,6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RandomOrOrder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随机组（随机或是按顺序）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body1.prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body2.prefab</t>
-  </si>
-  <si>
-    <t>body3.prefab</t>
-  </si>
-  <si>
-    <t>body4.prefab</t>
-  </si>
-  <si>
-    <t>body5.prefab</t>
-  </si>
-  <si>
-    <t>body6.prefab</t>
-  </si>
-  <si>
-    <t>body7.prefab</t>
-  </si>
-  <si>
-    <t>body8.prefab</t>
-  </si>
-  <si>
-    <t>Path</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>路径</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>body2</t>
-  </si>
-  <si>
-    <t>body3</t>
-  </si>
-  <si>
-    <t>body4</t>
-  </si>
-  <si>
-    <t>body5</t>
-  </si>
-  <si>
-    <t>body6</t>
-  </si>
-  <si>
-    <t>body7</t>
-  </si>
-  <si>
-    <t>body8</t>
-  </si>
-  <si>
-    <t>#number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[RespawnPoint.Id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[string:Skin.Id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CharacterClass.Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[UnitGroup.Id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[Unit.Id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单位组列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lev</t>
+    <t>重生点8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body:2</t>
+  </si>
+  <si>
+    <t>body:3</t>
+  </si>
+  <si>
+    <t>body:4</t>
+  </si>
+  <si>
+    <t>body:5</t>
+  </si>
+  <si>
+    <t>body:6</t>
+  </si>
+  <si>
+    <t>body:7</t>
+  </si>
+  <si>
+    <t>body:8</t>
+  </si>
+  <si>
+    <t>body:9</t>
+  </si>
+  <si>
+    <t>body9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>body9prefab</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -816,7 +862,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -833,7 +879,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -904,7 +950,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>75</v>
@@ -928,7 +974,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -941,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -955,16 +1001,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -986,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,13 +1046,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,13 +1060,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,13 +1074,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,13 +1088,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,13 +1102,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,13 +1116,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1084,13 +1130,13 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,13 +1144,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1134,13 +1180,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,7 +1200,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1165,10 +1211,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1176,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1190,13 +1236,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1207,56 +1253,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="83.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.5" customWidth="1"/>
-    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="91.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>65</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1268,7 +1314,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -1277,10 +1323,10 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1291,44 +1337,50 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
-      </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="H4" t="b">
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
@@ -1339,19 +1391,25 @@
       <c r="A5">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="b">
+      <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="H5" t="b">
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
@@ -1362,19 +1420,25 @@
       <c r="A6">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="b">
+      <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="H6" t="b">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
@@ -1385,19 +1449,25 @@
       <c r="A7">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="b">
+      <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="H7" t="b">
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
@@ -1408,19 +1478,25 @@
       <c r="A8">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="b">
+      <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8" t="b">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
@@ -1431,19 +1507,25 @@
       <c r="A9">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="b">
+      <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="H9" t="b">
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
@@ -1454,28 +1536,64 @@
       <c r="A10">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="b">
+      <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="H10" t="b">
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -1484,7 +1602,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1496,24 +1614,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1524,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1532,10 +1650,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1543,10 +1661,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1554,10 +1672,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1565,10 +1683,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1576,10 +1694,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1587,10 +1705,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1614,15 +1732,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1633,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1725,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238664E5-9C8B-4067-95CA-990B4C124D9B}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1740,35 +1858,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1776,10 +1894,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1787,10 +1905,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1798,10 +1916,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1809,10 +1927,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1820,10 +1938,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1831,10 +1949,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1842,10 +1960,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1853,10 +1971,21 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>